<commit_message>
[#PAB-232] remove partially left-over 'sheet_names' concept in ingest endpoint
</commit_message>
<xml_diff>
--- a/tests/controller_tests/resources/test_file.xlsx
+++ b/tests/controller_tests/resources/test_file.xlsx
@@ -1,19 +1,20 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26130"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-prototype-api\tests\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DobbsC\PycharmProjects\funding-service-design-post-award-data-store\tests\controller_tests\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78F4303E-DD7A-4953-9F75-33178E92EEF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46375E43-6FD9-466C-9B13-5683FD48CFBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="750" yWindow="5715" windowWidth="20265" windowHeight="14985" xr2:uid="{C0D4C5D0-1142-46FF-8442-C7DBDEDE0B49}"/>
+    <workbookView xWindow="6105" yWindow="4035" windowWidth="37275" windowHeight="14040" activeTab="1" xr2:uid="{C0D4C5D0-1142-46FF-8442-C7DBDEDE0B49}"/>
   </bookViews>
   <sheets>
     <sheet name="TestSheet" sheetId="1" r:id="rId1"/>
+    <sheet name="Another Sheet" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="7">
   <si>
     <t>Field 1</t>
   </si>
@@ -54,6 +55,9 @@
   </si>
   <si>
     <t>C</t>
+  </si>
+  <si>
+    <t>Data</t>
   </si>
 </sst>
 </file>
@@ -408,8 +412,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F2168DF-01DE-4105-A347-1EAE09D39ACD}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -469,6 +473,53 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AAB3018F-9BAF-4D4D-9F61-8222798737D2}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B4" sqref="B4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B4" t="s">
+        <v>6</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=docMetadata/LabelInfo.xml><?xml version="1.0" encoding="utf-8"?>
 <clbl:labelList xmlns:clbl="http://schemas.microsoft.com/office/2020/mipLabelMetadata">
   <clbl:label id="{95c71a0f-75e1-4c8f-90e2-641c9351dd98}" enabled="1" method="Standard" siteId="{3e0088dc-0629-4ae6-aa8c-813e7a296f50}" contentBits="2" removed="0"/>

</xml_diff>